<commit_message>
numpy finished, WPMTracker modifiziert
</commit_message>
<xml_diff>
--- a/Projects/WPMTracker/WPM.xlsx
+++ b/Projects/WPMTracker/WPM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="2490" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="1620" windowWidth="29040" windowHeight="16440" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="WPM" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="18">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -91,6 +91,28 @@
     </font>
     <font>
       <name val="Calibri"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
       <strike val="0"/>
       <color rgb="FF000000"/>
       <sz val="11"/>
@@ -103,12 +125,84 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="50">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9BC2E6"/>
+        <bgColor rgb="FF9BC2E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0CECE"/>
+        <bgColor rgb="FFD0CECE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D08E"/>
+        <bgColor rgb="FFA9D08E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDD5151"/>
+        <bgColor rgb="FFDD5151"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9BC2E6"/>
+        <bgColor rgb="FF9BC2E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0CECE"/>
+        <bgColor rgb="FFD0CECE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D08E"/>
+        <bgColor rgb="FFA9D08E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDD5151"/>
+        <bgColor rgb="FFDD5151"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -327,7 +421,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -415,6 +509,28 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <right style="thick"/>
       <bottom style="thin"/>
     </border>
@@ -422,7 +538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
@@ -511,9 +627,6 @@
     <xf numFmtId="0" fontId="9" fillId="22" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="23" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -532,6 +645,9 @@
     <xf numFmtId="0" fontId="11" fillId="28" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="29" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -541,7 +657,7 @@
     <xf numFmtId="0" fontId="10" fillId="31" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="32" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -563,6 +679,48 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="37" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="38" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="39" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="40" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="39" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="41" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="42" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="43" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="44" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="45" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="46" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="45" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="47" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="48" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="49" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -910,8 +1068,8 @@
   </sheetPr>
   <dimension ref="A1:I4434"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:I17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1418,732 +1576,956 @@
       <c r="C16" s="29" t="n">
         <v>103</v>
       </c>
-      <c r="D16" s="30" t="inlineStr">
+      <c r="D16" s="40" t="inlineStr">
         <is>
-          <t>95.9</t>
+          <t>95.90</t>
         </is>
       </c>
-      <c r="E16" s="31" t="n">
+      <c r="E16" s="30" t="n">
         <v>536</v>
       </c>
-      <c r="F16" s="32" t="n">
+      <c r="F16" s="31" t="n">
         <v>515</v>
       </c>
-      <c r="G16" s="33" t="n">
+      <c r="G16" s="32" t="n">
         <v>21</v>
       </c>
-      <c r="H16" s="32" t="n">
+      <c r="H16" s="31" t="n">
         <v>96</v>
       </c>
-      <c r="I16" s="33" t="n">
+      <c r="I16" s="32" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="41" t="n">
+      <c r="A17" s="33" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="42" t="n">
+      <c r="B17" s="34" t="n">
         <v>44312.56297086806</v>
       </c>
-      <c r="C17" s="43" t="n">
+      <c r="C17" s="35" t="n">
         <v>96</v>
       </c>
-      <c r="D17" s="44" t="inlineStr">
+      <c r="D17" s="36" t="inlineStr">
         <is>
           <t>93.36</t>
         </is>
       </c>
-      <c r="E17" s="45" t="n">
+      <c r="E17" s="37" t="n">
         <v>512</v>
       </c>
-      <c r="F17" s="46" t="n">
+      <c r="F17" s="38" t="n">
         <v>478</v>
       </c>
-      <c r="G17" s="47" t="n">
+      <c r="G17" s="39" t="n">
         <v>34</v>
       </c>
-      <c r="H17" s="46" t="n">
+      <c r="H17" s="38" t="n">
         <v>93</v>
       </c>
-      <c r="I17" s="47" t="n">
+      <c r="I17" s="39" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="41" t="n">
+      <c r="A18" s="33" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="42" t="n">
+      <c r="B18" s="34" t="n">
         <v>44312.61090046296</v>
       </c>
-      <c r="C18" s="43" t="n">
+      <c r="C18" s="35" t="n">
         <v>102</v>
       </c>
-      <c r="D18" s="44" t="inlineStr">
+      <c r="D18" s="36" t="inlineStr">
         <is>
           <t>96.21</t>
         </is>
       </c>
-      <c r="E18" s="45" t="n">
+      <c r="E18" s="37" t="n">
         <v>522</v>
       </c>
-      <c r="F18" s="46" t="n">
+      <c r="F18" s="38" t="n">
         <v>508</v>
       </c>
-      <c r="G18" s="47" t="n">
+      <c r="G18" s="39" t="n">
         <v>14</v>
       </c>
-      <c r="H18" s="46" t="n">
+      <c r="H18" s="38" t="n">
         <v>92</v>
       </c>
-      <c r="I18" s="47" t="n">
+      <c r="I18" s="39" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="41" t="n">
+      <c r="A19" s="33" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="42" t="n">
+      <c r="B19" s="34" t="n">
         <v>44312.64613854167</v>
       </c>
-      <c r="C19" s="43" t="n">
+      <c r="C19" s="35" t="n">
         <v>93</v>
       </c>
-      <c r="D19" s="44" t="inlineStr">
+      <c r="D19" s="36" t="inlineStr">
         <is>
           <t>92.05</t>
         </is>
       </c>
-      <c r="E19" s="45" t="n">
+      <c r="E19" s="37" t="n">
         <v>493</v>
       </c>
-      <c r="F19" s="46" t="n">
+      <c r="F19" s="38" t="n">
         <v>463</v>
       </c>
-      <c r="G19" s="47" t="n">
+      <c r="G19" s="39" t="n">
         <v>30</v>
       </c>
-      <c r="H19" s="46" t="n">
+      <c r="H19" s="38" t="n">
         <v>86</v>
       </c>
-      <c r="I19" s="47" t="n">
+      <c r="I19" s="39" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="41" t="n">
+      <c r="A20" s="33" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="42" t="n">
+      <c r="B20" s="34" t="n">
         <v>44312.64858355324</v>
       </c>
-      <c r="C20" s="43" t="n">
+      <c r="C20" s="35" t="n">
         <v>95</v>
       </c>
-      <c r="D20" s="44" t="inlineStr">
+      <c r="D20" s="36" t="inlineStr">
         <is>
           <t>93.68</t>
         </is>
       </c>
-      <c r="E20" s="45" t="n">
+      <c r="E20" s="37" t="n">
         <v>499</v>
       </c>
-      <c r="F20" s="46" t="n">
+      <c r="F20" s="38" t="n">
         <v>474</v>
       </c>
-      <c r="G20" s="47" t="n">
+      <c r="G20" s="39" t="n">
         <v>25</v>
       </c>
-      <c r="H20" s="46" t="n">
+      <c r="H20" s="38" t="n">
         <v>90</v>
       </c>
-      <c r="I20" s="47" t="n">
+      <c r="I20" s="39" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="41" t="n">
+      <c r="A21" s="33" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="42" t="n">
+      <c r="B21" s="34" t="n">
         <v>44312.67528114584</v>
       </c>
-      <c r="C21" s="43" t="n">
+      <c r="C21" s="35" t="n">
         <v>99</v>
       </c>
-      <c r="D21" s="44" t="inlineStr">
+      <c r="D21" s="36" t="inlineStr">
         <is>
           <t>95.01</t>
         </is>
       </c>
-      <c r="E21" s="45" t="n">
+      <c r="E21" s="37" t="n">
         <v>514</v>
       </c>
-      <c r="F21" s="46" t="n">
+      <c r="F21" s="38" t="n">
         <v>495</v>
       </c>
-      <c r="G21" s="47" t="n">
+      <c r="G21" s="39" t="n">
         <v>19</v>
       </c>
-      <c r="H21" s="46" t="n">
+      <c r="H21" s="38" t="n">
         <v>89</v>
       </c>
-      <c r="I21" s="47" t="n">
+      <c r="I21" s="39" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="41" t="n">
+      <c r="A22" s="33" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="42" t="n">
+      <c r="B22" s="34" t="n">
         <v>44313.48644244213</v>
       </c>
-      <c r="C22" s="43" t="n">
+      <c r="C22" s="35" t="n">
         <v>92</v>
       </c>
-      <c r="D22" s="44" t="inlineStr">
+      <c r="D22" s="36" t="inlineStr">
         <is>
           <t>89.51</t>
         </is>
       </c>
-      <c r="E22" s="45" t="n">
+      <c r="E22" s="37" t="n">
         <v>509</v>
       </c>
-      <c r="F22" s="46" t="n">
+      <c r="F22" s="38" t="n">
         <v>461</v>
       </c>
-      <c r="G22" s="47" t="n">
+      <c r="G22" s="39" t="n">
         <v>48</v>
       </c>
-      <c r="H22" s="46" t="n">
+      <c r="H22" s="38" t="n">
         <v>81</v>
       </c>
-      <c r="I22" s="47" t="n">
+      <c r="I22" s="39" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="41" t="n">
+      <c r="A23" s="33" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="42" t="n">
+      <c r="B23" s="34" t="n">
         <v>44313.71834622685</v>
       </c>
-      <c r="C23" s="43" t="n">
+      <c r="C23" s="35" t="n">
         <v>87</v>
       </c>
-      <c r="D23" s="44" t="inlineStr">
+      <c r="D23" s="36" t="inlineStr">
         <is>
           <t>94.37</t>
         </is>
       </c>
-      <c r="E23" s="45" t="n">
+      <c r="E23" s="37" t="n">
         <v>446</v>
       </c>
-      <c r="F23" s="46" t="n">
+      <c r="F23" s="38" t="n">
         <v>436</v>
       </c>
-      <c r="G23" s="47" t="n">
+      <c r="G23" s="39" t="n">
         <v>10</v>
       </c>
-      <c r="H23" s="46" t="n">
+      <c r="H23" s="38" t="n">
         <v>83</v>
       </c>
-      <c r="I23" s="47" t="n">
+      <c r="I23" s="39" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="41" t="n">
+      <c r="A24" s="33" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="42" t="n">
+      <c r="B24" s="34" t="n">
         <v>44313.76619</v>
       </c>
-      <c r="C24" s="43" t="n">
+      <c r="C24" s="35" t="n">
         <v>91</v>
       </c>
-      <c r="D24" s="44" t="inlineStr">
+      <c r="D24" s="36" t="inlineStr">
         <is>
           <t>92.64</t>
         </is>
       </c>
-      <c r="E24" s="45" t="n">
+      <c r="E24" s="37" t="n">
         <v>484</v>
       </c>
-      <c r="F24" s="46" t="n">
+      <c r="F24" s="38" t="n">
         <v>453</v>
       </c>
-      <c r="G24" s="47" t="n">
+      <c r="G24" s="39" t="n">
         <v>31</v>
       </c>
-      <c r="H24" s="46" t="n">
+      <c r="H24" s="38" t="n">
         <v>86</v>
       </c>
-      <c r="I24" s="47" t="n">
+      <c r="I24" s="39" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="41" t="n">
+      <c r="A25" s="33" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="42" t="n">
+      <c r="B25" s="34" t="n">
         <v>44314.46535142361</v>
       </c>
-      <c r="C25" s="43" t="n">
+      <c r="C25" s="35" t="n">
         <v>97</v>
       </c>
-      <c r="D25" s="44" t="inlineStr">
+      <c r="D25" s="36" t="inlineStr">
         <is>
           <t>95.12</t>
         </is>
       </c>
-      <c r="E25" s="45" t="n">
+      <c r="E25" s="37" t="n">
         <v>502</v>
       </c>
-      <c r="F25" s="46" t="n">
+      <c r="F25" s="38" t="n">
         <v>487</v>
       </c>
-      <c r="G25" s="47" t="n">
+      <c r="G25" s="39" t="n">
         <v>15</v>
       </c>
-      <c r="H25" s="46" t="n">
+      <c r="H25" s="38" t="n">
         <v>93</v>
       </c>
-      <c r="I25" s="47" t="n">
+      <c r="I25" s="39" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="41" t="n">
+      <c r="A26" s="33" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="42" t="n">
+      <c r="B26" s="34" t="n">
         <v>44314.46615027777</v>
       </c>
-      <c r="C26" s="43" t="n">
+      <c r="C26" s="35" t="n">
         <v>95</v>
       </c>
-      <c r="D26" s="44" t="inlineStr">
+      <c r="D26" s="36" t="inlineStr">
         <is>
           <t>97.14</t>
         </is>
       </c>
-      <c r="E26" s="45" t="n">
+      <c r="E26" s="37" t="n">
         <v>482</v>
       </c>
-      <c r="F26" s="46" t="n">
+      <c r="F26" s="38" t="n">
         <v>475</v>
       </c>
-      <c r="G26" s="47" t="n">
+      <c r="G26" s="39" t="n">
         <v>7</v>
       </c>
-      <c r="H26" s="46" t="n">
+      <c r="H26" s="38" t="n">
         <v>86</v>
       </c>
-      <c r="I26" s="47" t="n">
+      <c r="I26" s="39" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="41" t="n">
+      <c r="A27" s="33" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="42" t="n">
+      <c r="B27" s="34" t="n">
         <v>44314.46709310186</v>
       </c>
-      <c r="C27" s="43" t="n">
+      <c r="C27" s="35" t="n">
         <v>94</v>
       </c>
-      <c r="D27" s="44" t="inlineStr">
+      <c r="D27" s="36" t="inlineStr">
         <is>
           <t>93.45</t>
         </is>
       </c>
-      <c r="E27" s="45" t="n">
+      <c r="E27" s="37" t="n">
         <v>498</v>
       </c>
-      <c r="F27" s="46" t="n">
+      <c r="F27" s="38" t="n">
         <v>471</v>
       </c>
-      <c r="G27" s="47" t="n">
+      <c r="G27" s="39" t="n">
         <v>27</v>
       </c>
-      <c r="H27" s="46" t="n">
+      <c r="H27" s="38" t="n">
         <v>87</v>
       </c>
-      <c r="I27" s="47" t="n">
+      <c r="I27" s="39" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="41" t="n">
+      <c r="A28" s="33" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="42" t="n">
+      <c r="B28" s="34" t="n">
         <v>44314.46806174768</v>
       </c>
-      <c r="C28" s="43" t="n">
+      <c r="C28" s="35" t="n">
         <v>90</v>
       </c>
-      <c r="D28" s="44" t="inlineStr">
+      <c r="D28" s="36" t="inlineStr">
         <is>
           <t>92.06</t>
         </is>
       </c>
-      <c r="E28" s="45" t="n">
+      <c r="E28" s="37" t="n">
         <v>485</v>
       </c>
-      <c r="F28" s="46" t="n">
+      <c r="F28" s="38" t="n">
         <v>452</v>
       </c>
-      <c r="G28" s="47" t="n">
+      <c r="G28" s="39" t="n">
         <v>33</v>
       </c>
-      <c r="H28" s="46" t="n">
+      <c r="H28" s="38" t="n">
         <v>81</v>
       </c>
-      <c r="I28" s="47" t="n">
+      <c r="I28" s="39" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="41" t="n">
+      <c r="A29" s="33" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="42" t="n">
+      <c r="B29" s="34" t="n">
         <v>44314.54006215278</v>
       </c>
-      <c r="C29" s="43" t="n">
+      <c r="C29" s="35" t="n">
         <v>93</v>
       </c>
-      <c r="D29" s="44" t="inlineStr">
+      <c r="D29" s="36" t="inlineStr">
         <is>
           <t>94.13</t>
         </is>
       </c>
-      <c r="E29" s="45" t="n">
+      <c r="E29" s="37" t="n">
         <v>485</v>
       </c>
-      <c r="F29" s="46" t="n">
+      <c r="F29" s="38" t="n">
         <v>465</v>
       </c>
-      <c r="G29" s="47" t="n">
+      <c r="G29" s="39" t="n">
         <v>20</v>
       </c>
-      <c r="H29" s="46" t="n">
+      <c r="H29" s="38" t="n">
         <v>83</v>
       </c>
-      <c r="I29" s="47" t="n">
+      <c r="I29" s="39" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="41" t="n">
+      <c r="A30" s="33" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="42" t="n">
+      <c r="B30" s="34" t="n">
         <v>44314.703115</v>
       </c>
-      <c r="C30" s="43" t="n">
+      <c r="C30" s="35" t="n">
         <v>87</v>
       </c>
-      <c r="D30" s="44" t="inlineStr">
+      <c r="D30" s="36" t="inlineStr">
         <is>
           <t>94.16</t>
         </is>
       </c>
-      <c r="E30" s="45" t="n">
+      <c r="E30" s="37" t="n">
         <v>450</v>
       </c>
-      <c r="F30" s="46" t="n">
+      <c r="F30" s="38" t="n">
         <v>435</v>
       </c>
-      <c r="G30" s="47" t="n">
+      <c r="G30" s="39" t="n">
         <v>15</v>
       </c>
-      <c r="H30" s="46" t="n">
+      <c r="H30" s="38" t="n">
         <v>76</v>
       </c>
-      <c r="I30" s="47" t="n">
+      <c r="I30" s="39" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="41" t="n">
+      <c r="A31" s="33" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="42" t="n">
+      <c r="B31" s="34" t="n">
         <v>44314.7040015625</v>
       </c>
-      <c r="C31" s="43" t="n">
+      <c r="C31" s="35" t="n">
         <v>89</v>
       </c>
-      <c r="D31" s="44" t="inlineStr">
+      <c r="D31" s="36" t="inlineStr">
         <is>
           <t>95.28</t>
         </is>
       </c>
-      <c r="E31" s="45" t="n">
+      <c r="E31" s="37" t="n">
         <v>460</v>
       </c>
-      <c r="F31" s="46" t="n">
+      <c r="F31" s="38" t="n">
         <v>444</v>
       </c>
-      <c r="G31" s="47" t="n">
+      <c r="G31" s="39" t="n">
         <v>16</v>
       </c>
-      <c r="H31" s="46" t="n">
+      <c r="H31" s="38" t="n">
         <v>84</v>
       </c>
-      <c r="I31" s="47" t="n">
+      <c r="I31" s="39" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="41" t="n">
+      <c r="A32" s="33" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="42" t="n">
+      <c r="B32" s="34" t="n">
         <v>44314.8126249537</v>
       </c>
-      <c r="C32" s="43" t="n">
+      <c r="C32" s="35" t="n">
         <v>101</v>
       </c>
-      <c r="D32" s="44" t="inlineStr">
+      <c r="D32" s="36" t="inlineStr">
         <is>
           <t>97.68</t>
         </is>
       </c>
-      <c r="E32" s="45" t="n">
+      <c r="E32" s="37" t="n">
         <v>512</v>
       </c>
-      <c r="F32" s="46" t="n">
+      <c r="F32" s="38" t="n">
         <v>506</v>
       </c>
-      <c r="G32" s="47" t="n">
+      <c r="G32" s="39" t="n">
         <v>6</v>
       </c>
-      <c r="H32" s="46" t="n">
+      <c r="H32" s="38" t="n">
         <v>90</v>
       </c>
-      <c r="I32" s="47" t="n">
+      <c r="I32" s="39" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="41" t="n">
+      <c r="A33" s="33" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="42" t="n">
+      <c r="B33" s="34" t="n">
         <v>44314.92988149306</v>
       </c>
-      <c r="C33" s="43" t="n">
+      <c r="C33" s="35" t="n">
         <v>95</v>
       </c>
-      <c r="D33" s="44" t="inlineStr">
+      <c r="D33" s="36" t="inlineStr">
         <is>
           <t>95.59</t>
         </is>
       </c>
-      <c r="E33" s="45" t="n">
+      <c r="E33" s="37" t="n">
         <v>492</v>
       </c>
-      <c r="F33" s="46" t="n">
+      <c r="F33" s="38" t="n">
         <v>477</v>
       </c>
-      <c r="G33" s="47" t="n">
+      <c r="G33" s="39" t="n">
         <v>15</v>
       </c>
-      <c r="H33" s="46" t="n">
+      <c r="H33" s="38" t="n">
         <v>86</v>
       </c>
-      <c r="I33" s="47" t="n">
+      <c r="I33" s="39" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="41" t="n">
+      <c r="A34" s="33" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="42" t="n">
+      <c r="B34" s="34" t="n">
         <v>44315.49031497685</v>
       </c>
-      <c r="C34" s="43" t="n">
+      <c r="C34" s="35" t="n">
         <v>93</v>
       </c>
-      <c r="D34" s="44" t="inlineStr">
+      <c r="D34" s="36" t="inlineStr">
         <is>
           <t>91.32</t>
         </is>
       </c>
-      <c r="E34" s="45" t="n">
+      <c r="E34" s="37" t="n">
         <v>499</v>
       </c>
-      <c r="F34" s="46" t="n">
+      <c r="F34" s="38" t="n">
         <v>463</v>
       </c>
-      <c r="G34" s="47" t="n">
+      <c r="G34" s="39" t="n">
         <v>36</v>
       </c>
-      <c r="H34" s="46" t="n">
+      <c r="H34" s="38" t="n">
         <v>86</v>
       </c>
-      <c r="I34" s="47" t="n">
+      <c r="I34" s="39" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="41" t="n">
+      <c r="A35" s="33" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="42" t="n">
+      <c r="B35" s="34" t="n">
         <v>44315.50159837963</v>
       </c>
-      <c r="C35" s="43" t="n">
+      <c r="C35" s="35" t="n">
         <v>87</v>
       </c>
-      <c r="D35" s="44" t="inlineStr">
+      <c r="D35" s="36" t="inlineStr">
         <is>
           <t>91.93</t>
         </is>
       </c>
-      <c r="E35" s="45" t="n">
+      <c r="E35" s="37" t="n">
         <v>450</v>
       </c>
-      <c r="F35" s="46" t="n">
+      <c r="F35" s="38" t="n">
         <v>433</v>
       </c>
-      <c r="G35" s="47" t="n">
+      <c r="G35" s="39" t="n">
         <v>17</v>
       </c>
-      <c r="H35" s="46" t="n">
+      <c r="H35" s="38" t="n">
         <v>79</v>
       </c>
-      <c r="I35" s="47" t="n">
+      <c r="I35" s="39" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="41" t="n">
+      <c r="A36" s="33" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="42" t="n">
+      <c r="B36" s="34" t="n">
         <v>44315.5024756713</v>
       </c>
-      <c r="C36" s="43" t="n">
+      <c r="C36" s="35" t="n">
         <v>90</v>
       </c>
-      <c r="D36" s="44" t="inlineStr">
+      <c r="D36" s="36" t="inlineStr">
         <is>
           <t>90.18</t>
         </is>
       </c>
-      <c r="E36" s="45" t="n">
+      <c r="E36" s="37" t="n">
         <v>492</v>
       </c>
-      <c r="F36" s="46" t="n">
+      <c r="F36" s="38" t="n">
         <v>450</v>
       </c>
-      <c r="G36" s="47" t="n">
+      <c r="G36" s="39" t="n">
         <v>42</v>
       </c>
-      <c r="H36" s="46" t="n">
+      <c r="H36" s="38" t="n">
         <v>82</v>
       </c>
-      <c r="I36" s="47" t="n">
+      <c r="I36" s="39" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="41" t="n">
+      <c r="A37" s="33" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="42" t="n">
+      <c r="B37" s="34" t="n">
         <v>44315.50328333333</v>
       </c>
-      <c r="C37" s="43" t="n">
+      <c r="C37" s="35" t="n">
         <v>89</v>
       </c>
-      <c r="D37" s="44" t="inlineStr">
+      <c r="D37" s="36" t="inlineStr">
         <is>
           <t>88.14</t>
         </is>
       </c>
-      <c r="E37" s="45" t="n">
+      <c r="E37" s="37" t="n">
         <v>495</v>
       </c>
-      <c r="F37" s="46" t="n">
+      <c r="F37" s="38" t="n">
         <v>446</v>
       </c>
-      <c r="G37" s="47" t="n">
+      <c r="G37" s="39" t="n">
         <v>49</v>
       </c>
-      <c r="H37" s="46" t="n">
+      <c r="H37" s="38" t="n">
         <v>79</v>
       </c>
-      <c r="I37" s="47" t="n">
+      <c r="I37" s="39" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="41" t="n">
+      <c r="A38" s="33" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="42" t="n">
-        <v>44315.66456087104</v>
-      </c>
-      <c r="C38" s="43" t="n">
+      <c r="B38" s="34" t="n">
+        <v>44315.66456086806</v>
+      </c>
+      <c r="C38" s="35" t="n">
         <v>92</v>
       </c>
-      <c r="D38" s="44" t="inlineStr">
+      <c r="D38" s="36" t="inlineStr">
         <is>
           <t>96.45</t>
         </is>
       </c>
-      <c r="E38" s="45" t="n">
+      <c r="E38" s="37" t="n">
         <v>474</v>
       </c>
-      <c r="F38" s="46" t="n">
+      <c r="F38" s="38" t="n">
         <v>462</v>
       </c>
-      <c r="G38" s="47" t="n">
+      <c r="G38" s="39" t="n">
         <v>12</v>
       </c>
-      <c r="H38" s="46" t="n">
+      <c r="H38" s="38" t="n">
         <v>86</v>
       </c>
-      <c r="I38" s="47" t="n">
+      <c r="I38" s="39" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="39">
-      <c r="B39" s="12" t="n"/>
+      <c r="A39" s="33" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="34" t="n">
+        <v>44316.44882023148</v>
+      </c>
+      <c r="C39" s="35" t="n">
+        <v>92</v>
+      </c>
+      <c r="D39" s="36" t="inlineStr">
+        <is>
+          <t>92.91</t>
+        </is>
+      </c>
+      <c r="E39" s="37" t="n">
+        <v>484</v>
+      </c>
+      <c r="F39" s="38" t="n">
+        <v>459</v>
+      </c>
+      <c r="G39" s="39" t="n">
+        <v>25</v>
+      </c>
+      <c r="H39" s="38" t="n">
+        <v>84</v>
+      </c>
+      <c r="I39" s="39" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="40">
-      <c r="B40" s="12" t="n"/>
+      <c r="A40" s="33" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="34" t="n">
+        <v>44316.45132209491</v>
+      </c>
+      <c r="C40" s="35" t="n">
+        <v>95</v>
+      </c>
+      <c r="D40" s="36" t="inlineStr">
+        <is>
+          <t>93.15</t>
+        </is>
+      </c>
+      <c r="E40" s="37" t="n">
+        <v>507</v>
+      </c>
+      <c r="F40" s="38" t="n">
+        <v>476</v>
+      </c>
+      <c r="G40" s="39" t="n">
+        <v>31</v>
+      </c>
+      <c r="H40" s="38" t="n">
+        <v>83</v>
+      </c>
+      <c r="I40" s="39" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="41">
-      <c r="B41" s="12" t="n"/>
+      <c r="A41" s="33" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="34" t="n">
+        <v>44316.47396231481</v>
+      </c>
+      <c r="C41" s="35" t="n">
+        <v>102</v>
+      </c>
+      <c r="D41" s="36" t="inlineStr">
+        <is>
+          <t>96.40</t>
+        </is>
+      </c>
+      <c r="E41" s="37" t="n">
+        <v>521</v>
+      </c>
+      <c r="F41" s="38" t="n">
+        <v>509</v>
+      </c>
+      <c r="G41" s="39" t="n">
+        <v>12</v>
+      </c>
+      <c r="H41" s="38" t="n">
+        <v>94</v>
+      </c>
+      <c r="I41" s="39" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="42">
-      <c r="B42" s="12" t="n"/>
+      <c r="A42" s="41" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="42" t="n">
+        <v>44316.47610799769</v>
+      </c>
+      <c r="C42" s="43" t="n">
+        <v>99</v>
+      </c>
+      <c r="D42" s="44" t="inlineStr">
+        <is>
+          <t>94.12</t>
+        </is>
+      </c>
+      <c r="E42" s="45" t="n">
+        <v>521</v>
+      </c>
+      <c r="F42" s="46" t="n">
+        <v>496</v>
+      </c>
+      <c r="G42" s="47" t="n">
+        <v>25</v>
+      </c>
+      <c r="H42" s="46" t="n">
+        <v>85</v>
+      </c>
+      <c r="I42" s="47" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="43">
-      <c r="B43" s="12" t="n"/>
+      <c r="A43" s="41" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="42" t="n">
+        <v>44316.6135946875</v>
+      </c>
+      <c r="C43" s="43" t="n">
+        <v>104</v>
+      </c>
+      <c r="D43" s="44" t="inlineStr">
+        <is>
+          <t>93.87</t>
+        </is>
+      </c>
+      <c r="E43" s="45" t="n">
+        <v>546</v>
+      </c>
+      <c r="F43" s="46" t="n">
+        <v>521</v>
+      </c>
+      <c r="G43" s="47" t="n">
+        <v>25</v>
+      </c>
+      <c r="H43" s="46" t="n">
+        <v>99</v>
+      </c>
+      <c r="I43" s="47" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="44">
-      <c r="B44" s="12" t="n"/>
+      <c r="A44" s="48" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="49" t="n">
+        <v>44316.68296237269</v>
+      </c>
+      <c r="C44" s="50" t="n">
+        <v>99</v>
+      </c>
+      <c r="D44" s="51" t="inlineStr">
+        <is>
+          <t>93.6</t>
+        </is>
+      </c>
+      <c r="E44" s="52" t="n">
+        <v>521</v>
+      </c>
+      <c r="F44" s="53" t="n">
+        <v>497</v>
+      </c>
+      <c r="G44" s="54" t="n">
+        <v>24</v>
+      </c>
+      <c r="H44" s="53" t="n">
+        <v>92</v>
+      </c>
+      <c r="I44" s="54" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="45">
-      <c r="B45" s="12" t="n"/>
+      <c r="A45" s="55" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="56" t="n">
+        <v>44316.85071179398</v>
+      </c>
+      <c r="C45" s="57" t="n">
+        <v>89</v>
+      </c>
+      <c r="D45" s="58" t="inlineStr">
+        <is>
+          <t>91.38</t>
+        </is>
+      </c>
+      <c r="E45" s="59" t="n">
+        <v>480</v>
+      </c>
+      <c r="F45" s="60" t="n">
+        <v>445</v>
+      </c>
+      <c r="G45" s="61" t="n">
+        <v>35</v>
+      </c>
+      <c r="H45" s="60" t="n">
+        <v>85</v>
+      </c>
+      <c r="I45" s="61" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="46">
-      <c r="B46" s="12" t="n"/>
+      <c r="A46" s="55" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="56" t="n">
+        <v>44316.92595446025</v>
+      </c>
+      <c r="C46" s="57" t="n">
+        <v>87</v>
+      </c>
+      <c r="D46" s="58" t="inlineStr">
+        <is>
+          <t>90.79</t>
+        </is>
+      </c>
+      <c r="E46" s="59" t="n">
+        <v>468</v>
+      </c>
+      <c r="F46" s="60" t="n">
+        <v>434</v>
+      </c>
+      <c r="G46" s="61" t="n">
+        <v>34</v>
+      </c>
+      <c r="H46" s="60" t="n">
+        <v>79</v>
+      </c>
+      <c r="I46" s="61" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="47">
       <c r="B47" s="12" t="n"/>

</xml_diff>

<commit_message>
new records, icons, hue module tests
</commit_message>
<xml_diff>
--- a/Projects/WPMTracker/WPM.xlsx
+++ b/Projects/WPMTracker/WPM.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="1620" windowWidth="29040" windowHeight="16440" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="WPM" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="WPM" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -18,7 +18,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="30">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -157,6 +157,28 @@
     </font>
     <font>
       <name val="Calibri"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
       <strike val="0"/>
       <color rgb="FF000000"/>
       <sz val="11"/>
@@ -169,12 +191,84 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="74">
+  <fills count="86">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9BC2E6"/>
+        <bgColor rgb="FF9BC2E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0CECE"/>
+        <bgColor rgb="FFD0CECE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D08E"/>
+        <bgColor rgb="FFA9D08E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDD5151"/>
+        <bgColor rgb="FFDD5151"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9BC2E6"/>
+        <bgColor rgb="FF9BC2E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0CECE"/>
+        <bgColor rgb="FFD0CECE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D08E"/>
+        <bgColor rgb="FFA9D08E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDD5151"/>
+        <bgColor rgb="FFDD5151"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -609,7 +703,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -763,6 +857,28 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <right style="thick"/>
       <bottom style="thin"/>
     </border>
@@ -770,7 +886,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
@@ -1037,6 +1153,48 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="73" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="74" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="75" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="76" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="75" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="77" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="78" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="79" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="80" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="81" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="82" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="81" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="83" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="84" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="85" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1385,7 +1543,7 @@
   <dimension ref="A1:I4434"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L53" sqref="L53"/>
+      <selection activeCell="A70" sqref="A70:I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3313,7 +3471,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="84" t="n">
-        <v>44319.53981607351</v>
+        <v>44319.53981607639</v>
       </c>
       <c r="C62" s="85" t="n">
         <v>98</v>
@@ -3340,49 +3498,469 @@
       </c>
     </row>
     <row r="63">
-      <c r="B63" s="12" t="n"/>
+      <c r="A63" s="83" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" s="84" t="n">
+        <v>44319.77530127315</v>
+      </c>
+      <c r="C63" s="85" t="n">
+        <v>96</v>
+      </c>
+      <c r="D63" s="86" t="inlineStr">
+        <is>
+          <t>95.06</t>
+        </is>
+      </c>
+      <c r="E63" s="87" t="n">
+        <v>503</v>
+      </c>
+      <c r="F63" s="88" t="n">
+        <v>481</v>
+      </c>
+      <c r="G63" s="89" t="n">
+        <v>22</v>
+      </c>
+      <c r="H63" s="88" t="n">
+        <v>91</v>
+      </c>
+      <c r="I63" s="89" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="64">
-      <c r="B64" s="12" t="n"/>
+      <c r="A64" s="83" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" s="84" t="n">
+        <v>44319.83623872685</v>
+      </c>
+      <c r="C64" s="85" t="n">
+        <v>98</v>
+      </c>
+      <c r="D64" s="86" t="inlineStr">
+        <is>
+          <t>97.21</t>
+        </is>
+      </c>
+      <c r="E64" s="87" t="n">
+        <v>496</v>
+      </c>
+      <c r="F64" s="88" t="n">
+        <v>488</v>
+      </c>
+      <c r="G64" s="89" t="n">
+        <v>8</v>
+      </c>
+      <c r="H64" s="88" t="n">
+        <v>87</v>
+      </c>
+      <c r="I64" s="89" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="65">
-      <c r="B65" s="12" t="n"/>
+      <c r="A65" s="83" t="n">
+        <v>65</v>
+      </c>
+      <c r="B65" s="84" t="n">
+        <v>44320.5101380324</v>
+      </c>
+      <c r="C65" s="85" t="n">
+        <v>96</v>
+      </c>
+      <c r="D65" s="86" t="inlineStr">
+        <is>
+          <t>91.76</t>
+        </is>
+      </c>
+      <c r="E65" s="87" t="n">
+        <v>511</v>
+      </c>
+      <c r="F65" s="88" t="n">
+        <v>479</v>
+      </c>
+      <c r="G65" s="89" t="n">
+        <v>32</v>
+      </c>
+      <c r="H65" s="88" t="n">
+        <v>87</v>
+      </c>
+      <c r="I65" s="89" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="66">
-      <c r="B66" s="12" t="n"/>
+      <c r="A66" s="90" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" s="91" t="n">
+        <v>44320.51111181713</v>
+      </c>
+      <c r="C66" s="92" t="n">
+        <v>97</v>
+      </c>
+      <c r="D66" s="93" t="inlineStr">
+        <is>
+          <t>91.51</t>
+        </is>
+      </c>
+      <c r="E66" s="94" t="n">
+        <v>523</v>
+      </c>
+      <c r="F66" s="95" t="n">
+        <v>485</v>
+      </c>
+      <c r="G66" s="96" t="n">
+        <v>38</v>
+      </c>
+      <c r="H66" s="95" t="n">
+        <v>89</v>
+      </c>
+      <c r="I66" s="96" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="67">
-      <c r="B67" s="12" t="n"/>
+      <c r="A67" s="90" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" s="91" t="n">
+        <v>44320.64885880787</v>
+      </c>
+      <c r="C67" s="92" t="n">
+        <v>107</v>
+      </c>
+      <c r="D67" s="93" t="inlineStr">
+        <is>
+          <t>96.74</t>
+        </is>
+      </c>
+      <c r="E67" s="94" t="n">
+        <v>546</v>
+      </c>
+      <c r="F67" s="95" t="n">
+        <v>534</v>
+      </c>
+      <c r="G67" s="96" t="n">
+        <v>12</v>
+      </c>
+      <c r="H67" s="95" t="n">
+        <v>95</v>
+      </c>
+      <c r="I67" s="96" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="68">
-      <c r="B68" s="12" t="n"/>
+      <c r="A68" s="90" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" s="91" t="n">
+        <v>44320.76720237268</v>
+      </c>
+      <c r="C68" s="92" t="n">
+        <v>104</v>
+      </c>
+      <c r="D68" s="93" t="inlineStr">
+        <is>
+          <t>98.29</t>
+        </is>
+      </c>
+      <c r="E68" s="94" t="n">
+        <v>523</v>
+      </c>
+      <c r="F68" s="95" t="n">
+        <v>518</v>
+      </c>
+      <c r="G68" s="96" t="n">
+        <v>5</v>
+      </c>
+      <c r="H68" s="95" t="n">
+        <v>95</v>
+      </c>
+      <c r="I68" s="96" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="69">
-      <c r="B69" s="12" t="n"/>
+      <c r="A69" s="90" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" s="91" t="n">
+        <v>44321.52213138889</v>
+      </c>
+      <c r="C69" s="92" t="n">
+        <v>93</v>
+      </c>
+      <c r="D69" s="93" t="inlineStr">
+        <is>
+          <t>92.64</t>
+        </is>
+      </c>
+      <c r="E69" s="94" t="n">
+        <v>497</v>
+      </c>
+      <c r="F69" s="95" t="n">
+        <v>466</v>
+      </c>
+      <c r="G69" s="96" t="n">
+        <v>31</v>
+      </c>
+      <c r="H69" s="95" t="n">
+        <v>84</v>
+      </c>
+      <c r="I69" s="96" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="70">
-      <c r="B70" s="12" t="n"/>
+      <c r="A70" s="97" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" s="98" t="n">
+        <v>44321.52332702546</v>
+      </c>
+      <c r="C70" s="99" t="n">
+        <v>106</v>
+      </c>
+      <c r="D70" s="100" t="inlineStr">
+        <is>
+          <t>98.88</t>
+        </is>
+      </c>
+      <c r="E70" s="101" t="n">
+        <v>533</v>
+      </c>
+      <c r="F70" s="102" t="n">
+        <v>528</v>
+      </c>
+      <c r="G70" s="103" t="n">
+        <v>5</v>
+      </c>
+      <c r="H70" s="102" t="n">
+        <v>99</v>
+      </c>
+      <c r="I70" s="103" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="71">
-      <c r="B71" s="12" t="n"/>
+      <c r="A71" s="97" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" s="98" t="n">
+        <v>44321.53082283565</v>
+      </c>
+      <c r="C71" s="99" t="n">
+        <v>91</v>
+      </c>
+      <c r="D71" s="100" t="inlineStr">
+        <is>
+          <t>93.03</t>
+        </is>
+      </c>
+      <c r="E71" s="101" t="n">
+        <v>483</v>
+      </c>
+      <c r="F71" s="102" t="n">
+        <v>454</v>
+      </c>
+      <c r="G71" s="103" t="n">
+        <v>29</v>
+      </c>
+      <c r="H71" s="102" t="n">
+        <v>84</v>
+      </c>
+      <c r="I71" s="103" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="72">
-      <c r="B72" s="12" t="n"/>
+      <c r="A72" s="97" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" s="98" t="n">
+        <v>44321.87667280093</v>
+      </c>
+      <c r="C72" s="99" t="n">
+        <v>98</v>
+      </c>
+      <c r="D72" s="100" t="inlineStr">
+        <is>
+          <t>95.5</t>
+        </is>
+      </c>
+      <c r="E72" s="101" t="n">
+        <v>502</v>
+      </c>
+      <c r="F72" s="102" t="n">
+        <v>488</v>
+      </c>
+      <c r="G72" s="103" t="n">
+        <v>14</v>
+      </c>
+      <c r="H72" s="102" t="n">
+        <v>87</v>
+      </c>
+      <c r="I72" s="103" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="73">
-      <c r="B73" s="12" t="n"/>
+      <c r="A73" s="97" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" s="98" t="n">
+        <v>44321.88015725694</v>
+      </c>
+      <c r="C73" s="99" t="n">
+        <v>97</v>
+      </c>
+      <c r="D73" s="100" t="inlineStr">
+        <is>
+          <t>90.84</t>
+        </is>
+      </c>
+      <c r="E73" s="101" t="n">
+        <v>530</v>
+      </c>
+      <c r="F73" s="102" t="n">
+        <v>486</v>
+      </c>
+      <c r="G73" s="103" t="n">
+        <v>44</v>
+      </c>
+      <c r="H73" s="102" t="n">
+        <v>85</v>
+      </c>
+      <c r="I73" s="103" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="74">
-      <c r="B74" s="12" t="n"/>
+      <c r="A74" s="97" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" s="98" t="n">
+        <v>44322.36507841435</v>
+      </c>
+      <c r="C74" s="99" t="n">
+        <v>91</v>
+      </c>
+      <c r="D74" s="100" t="inlineStr">
+        <is>
+          <t>90.42</t>
+        </is>
+      </c>
+      <c r="E74" s="101" t="n">
+        <v>494</v>
+      </c>
+      <c r="F74" s="102" t="n">
+        <v>453</v>
+      </c>
+      <c r="G74" s="103" t="n">
+        <v>41</v>
+      </c>
+      <c r="H74" s="102" t="n">
+        <v>79</v>
+      </c>
+      <c r="I74" s="103" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="75">
-      <c r="B75" s="12" t="n"/>
+      <c r="A75" s="97" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" s="98" t="n">
+        <v>44322.46600922454</v>
+      </c>
+      <c r="C75" s="99" t="n">
+        <v>99</v>
+      </c>
+      <c r="D75" s="100" t="inlineStr">
+        <is>
+          <t>95.74</t>
+        </is>
+      </c>
+      <c r="E75" s="101" t="n">
+        <v>511</v>
+      </c>
+      <c r="F75" s="102" t="n">
+        <v>494</v>
+      </c>
+      <c r="G75" s="103" t="n">
+        <v>17</v>
+      </c>
+      <c r="H75" s="102" t="n">
+        <v>87</v>
+      </c>
+      <c r="I75" s="103" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="76">
-      <c r="B76" s="12" t="n"/>
+      <c r="A76" s="97" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" s="98" t="n">
+        <v>44322.46773158565</v>
+      </c>
+      <c r="C76" s="99" t="n">
+        <v>93</v>
+      </c>
+      <c r="D76" s="100" t="inlineStr">
+        <is>
+          <t>95.89</t>
+        </is>
+      </c>
+      <c r="E76" s="101" t="n">
+        <v>478</v>
+      </c>
+      <c r="F76" s="102" t="n">
+        <v>467</v>
+      </c>
+      <c r="G76" s="103" t="n">
+        <v>11</v>
+      </c>
+      <c r="H76" s="102" t="n">
+        <v>82</v>
+      </c>
+      <c r="I76" s="103" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="77">
-      <c r="B77" s="12" t="n"/>
+      <c r="A77" s="97" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" s="98" t="n">
+        <v>44322.60005685057</v>
+      </c>
+      <c r="C77" s="99" t="n">
+        <v>97</v>
+      </c>
+      <c r="D77" s="100" t="inlineStr">
+        <is>
+          <t>94.55</t>
+        </is>
+      </c>
+      <c r="E77" s="101" t="n">
+        <v>505</v>
+      </c>
+      <c r="F77" s="102" t="n">
+        <v>486</v>
+      </c>
+      <c r="G77" s="103" t="n">
+        <v>19</v>
+      </c>
+      <c r="H77" s="102" t="n">
+        <v>89</v>
+      </c>
+      <c r="I77" s="103" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="78">
       <c r="B78" s="12" t="n"/>

</xml_diff>

<commit_message>
huges Update: Graphs in TK gepackt, GUI überarbeitet, Records eingefügt
</commit_message>
<xml_diff>
--- a/Projects/WPMTracker/WPM.xlsx
+++ b/Projects/WPMTracker/WPM.xlsx
@@ -5733,7 +5733,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="161" t="n">
-        <v>44335.44988772425</v>
+        <v>44335.44988771991</v>
       </c>
       <c r="C112" s="162" t="n">
         <v>103</v>
@@ -5760,16 +5760,128 @@
       </c>
     </row>
     <row r="113">
-      <c r="B113" s="12" t="n"/>
+      <c r="A113" s="160" t="n">
+        <v>112</v>
+      </c>
+      <c r="B113" s="161" t="n">
+        <v>44336.51063456018</v>
+      </c>
+      <c r="C113" s="162" t="n">
+        <v>96</v>
+      </c>
+      <c r="D113" s="163" t="inlineStr">
+        <is>
+          <t>91.92</t>
+        </is>
+      </c>
+      <c r="E113" s="164" t="n">
+        <v>508</v>
+      </c>
+      <c r="F113" s="165" t="n">
+        <v>478</v>
+      </c>
+      <c r="G113" s="166" t="n">
+        <v>30</v>
+      </c>
+      <c r="H113" s="165" t="n">
+        <v>89</v>
+      </c>
+      <c r="I113" s="166" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="114">
-      <c r="B114" s="12" t="n"/>
+      <c r="A114" s="160" t="n">
+        <v>113</v>
+      </c>
+      <c r="B114" s="161" t="n">
+        <v>44336.5121924537</v>
+      </c>
+      <c r="C114" s="162" t="n">
+        <v>102</v>
+      </c>
+      <c r="D114" s="163" t="inlineStr">
+        <is>
+          <t>95.32</t>
+        </is>
+      </c>
+      <c r="E114" s="164" t="n">
+        <v>530</v>
+      </c>
+      <c r="F114" s="165" t="n">
+        <v>509</v>
+      </c>
+      <c r="G114" s="166" t="n">
+        <v>21</v>
+      </c>
+      <c r="H114" s="165" t="n">
+        <v>96</v>
+      </c>
+      <c r="I114" s="166" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="115">
-      <c r="B115" s="12" t="n"/>
+      <c r="A115" s="160" t="n">
+        <v>114</v>
+      </c>
+      <c r="B115" s="161" t="n">
+        <v>44336.51312983796</v>
+      </c>
+      <c r="C115" s="162" t="n">
+        <v>106</v>
+      </c>
+      <c r="D115" s="163" t="inlineStr">
+        <is>
+          <t>95.14</t>
+        </is>
+      </c>
+      <c r="E115" s="164" t="n">
+        <v>548</v>
+      </c>
+      <c r="F115" s="165" t="n">
+        <v>528</v>
+      </c>
+      <c r="G115" s="166" t="n">
+        <v>20</v>
+      </c>
+      <c r="H115" s="165" t="n">
+        <v>101</v>
+      </c>
+      <c r="I115" s="166" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="116">
-      <c r="B116" s="12" t="n"/>
+      <c r="A116" s="160" t="n">
+        <v>115</v>
+      </c>
+      <c r="B116" s="161" t="n">
+        <v>44336.52231644037</v>
+      </c>
+      <c r="C116" s="162" t="n">
+        <v>103</v>
+      </c>
+      <c r="D116" s="163" t="inlineStr">
+        <is>
+          <t>96.98</t>
+        </is>
+      </c>
+      <c r="E116" s="164" t="n">
+        <v>522</v>
+      </c>
+      <c r="F116" s="165" t="n">
+        <v>514</v>
+      </c>
+      <c r="G116" s="166" t="n">
+        <v>8</v>
+      </c>
+      <c r="H116" s="165" t="n">
+        <v>92</v>
+      </c>
+      <c r="I116" s="166" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="117">
       <c r="B117" s="12" t="n"/>

</xml_diff>